<commit_message>
The excel file with production list now contains all the products from our supervisors
</commit_message>
<xml_diff>
--- a/Daily_Production_Plan.xlsx
+++ b/Daily_Production_Plan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="7">
   <si>
     <t>Daily production schedule</t>
   </si>
@@ -26,16 +26,16 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>P1</t>
+    <t>P3</t>
   </si>
   <si>
     <t>P2</t>
   </si>
   <si>
-    <t>P3</t>
+    <t>P4</t>
   </si>
   <si>
-    <t>P4</t>
+    <t>P1</t>
   </si>
 </sst>
 </file>
@@ -116,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -129,6 +129,13 @@
       <right/>
       <top/>
       <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -157,7 +164,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,11 +193,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,10 +290,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="F106" activeCellId="0" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -297,7 +316,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="7" customFormat="true" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -305,116 +324,804 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8" t="n">
+    <row r="3" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="8" t="n">
+    <row r="4" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="n">
+    <row r="5" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8" t="n">
+    <row r="10" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="8" t="n">
+    <row r="11" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="8" t="n">
+    <row r="12" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="8" t="n">
+    <row r="13" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="7" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="n">
+    <row r="14" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8" t="n">
+    <row r="15" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8" t="n">
+    <row r="16" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8" t="n">
+    <row r="17" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="18" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="7" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="7" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="7" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="7" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="7" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="7" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="7" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="7" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="7" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="7" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="7" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="7" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="7" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="7" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="7" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="7" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="7" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="7" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="7" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="7" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="7" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="7" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="7" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="7" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="7" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="7" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="7" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="7" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="7" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="7" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="7" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="7" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="7" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="7" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="7" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="7" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="7" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="7" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="7" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="7" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="7" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="7" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="7" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="7" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="7" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="7" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="7" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="7" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="7" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="7" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="7" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="7" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="7" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="7" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="7" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="7" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="7" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="7" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="7" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="7" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="7" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" s="7" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="7" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="7" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="7" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="7" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" s="7" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="7" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" s="7" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" s="7" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96" s="7" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" s="7" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" s="7" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="7" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100" s="7" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101" s="7" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" s="11" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>